<commit_message>
se coloca la cama en el consolidado de dietas de pacientes
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos-paci.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos-paci.xlsx
@@ -9,15 +9,15 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$L$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$L$2</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Relacion de Solicitudes</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nombre Completo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cama </t>
   </si>
   <si>
     <t>Sopa</t>
@@ -88,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -124,6 +127,43 @@
       <left style="thin">
         <color theme="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
       <right style="thin">
         <color theme="1"/>
       </right>
@@ -139,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -156,16 +196,19 @@
     <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -717,7 +760,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -726,11 +769,11 @@
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="4"/>
     <col customWidth="1" min="2" max="2" style="2" width="16.7109375"/>
     <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="22.8515625"/>
-    <col customWidth="1" min="4" max="4" style="1" width="24.7109375"/>
-    <col customWidth="1" min="5" max="9" style="1" width="17.28125"/>
-    <col customWidth="1" min="10" max="10" style="1" width="34.57421875"/>
-    <col customWidth="1" min="11" max="12" style="1" width="17.28125"/>
-    <col min="13" max="16384" style="1" width="11.421875"/>
+    <col customWidth="1" min="4" max="5" style="1" width="24.7109375"/>
+    <col customWidth="1" min="6" max="10" style="1" width="17.28125"/>
+    <col customWidth="1" min="11" max="11" style="1" width="34.57421875"/>
+    <col customWidth="1" min="12" max="13" style="1" width="17.28125"/>
+    <col min="14" max="16384" style="1" width="11.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="43.5" customHeight="1">
@@ -740,86 +783,90 @@
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" s="1" customFormat="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:K2"/>
+  <autoFilter ref="B2:L2"/>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="D1:L1"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
se añade la celda de torre a la relacion de solicitud de pacientes
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos-paci.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos-paci.xlsx
@@ -9,15 +9,15 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$L$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$M$2</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Relacion de Solicitudes</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nombre Completo</t>
+  </si>
+  <si>
+    <t>Torre</t>
   </si>
   <si>
     <t xml:space="preserve">Cama </t>
@@ -769,11 +772,11 @@
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="4"/>
     <col customWidth="1" min="2" max="2" style="2" width="16.7109375"/>
     <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="22.8515625"/>
-    <col customWidth="1" min="4" max="5" style="1" width="24.7109375"/>
-    <col customWidth="1" min="6" max="10" style="1" width="17.28125"/>
-    <col customWidth="1" min="11" max="11" style="1" width="34.57421875"/>
-    <col customWidth="1" min="12" max="13" style="1" width="17.28125"/>
-    <col min="14" max="16384" style="1" width="11.421875"/>
+    <col customWidth="1" min="4" max="6" style="1" width="24.7109375"/>
+    <col customWidth="1" min="7" max="11" style="1" width="17.28125"/>
+    <col customWidth="1" min="12" max="12" style="1" width="34.57421875"/>
+    <col customWidth="1" min="13" max="14" style="1" width="17.28125"/>
+    <col min="15" max="16384" style="1" width="11.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="43.5" customHeight="1">
@@ -790,8 +793,9 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="8"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" s="1" customFormat="1">
       <c r="A2" s="9" t="s">
@@ -830,43 +834,46 @@
       <c r="L2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:L2"/>
+  <autoFilter ref="B2:M2"/>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="D1:M1"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>